<commit_message>
Fully functional Code --features will be added soon
</commit_message>
<xml_diff>
--- a/Frontend/app/Backend/ANSC121.xlsx
+++ b/Frontend/app/Backend/ANSC121.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -46,6 +46,12 @@
       <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <color rgb="FF0D0D0D"/>
+      <sz val="8"/>
     </font>
   </fonts>
   <fills count="3">
@@ -77,7 +83,7 @@
       <protection locked="0" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -97,8 +103,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -480,8 +487,8 @@
   </sheetPr>
   <dimension ref="A1:AJ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="66" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView zoomScale="66" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.1796875" defaultRowHeight="16.5"/>
@@ -519,11 +526,11 @@
     <col width="58.81640625" bestFit="1" customWidth="1" style="1" min="33" max="33"/>
     <col width="29" bestFit="1" customWidth="1" style="1" min="34" max="34"/>
     <col width="22" customWidth="1" style="1" min="35" max="35"/>
-    <col width="9.1796875" customWidth="1" style="1" min="36" max="42"/>
-    <col width="9.1796875" customWidth="1" style="1" min="43" max="16384"/>
+    <col width="9.1796875" customWidth="1" style="1" min="36" max="49"/>
+    <col width="9.1796875" customWidth="1" style="1" min="50" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.75" customHeight="1" s="9">
+    <row r="1" ht="21.75" customHeight="1" s="10">
       <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Attendance Sheet</t>
@@ -571,7 +578,7 @@
       <c r="AI1" s="4" t="n"/>
       <c r="AJ1" s="8" t="n"/>
     </row>
-    <row r="2" ht="21.75" customHeight="1" s="9">
+    <row r="2" ht="21.75" customHeight="1" s="10">
       <c r="A2" s="3" t="inlineStr">
         <is>
           <t>21-1-00346</t>
@@ -617,7 +624,7 @@
       <c r="AI2" s="2" t="n"/>
       <c r="AJ2" s="8" t="n"/>
     </row>
-    <row r="3" ht="21.75" customHeight="1" s="9">
+    <row r="3" ht="21.75" customHeight="1" s="10">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>21-1-02625</t>
@@ -628,7 +635,9 @@
           <t xml:space="preserve">Braga, Maria </t>
         </is>
       </c>
-      <c r="C3" s="3" t="n"/>
+      <c r="C3" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
@@ -663,7 +672,7 @@
       <c r="AI3" s="2" t="n"/>
       <c r="AJ3" s="8" t="n"/>
     </row>
-    <row r="4" ht="21.75" customHeight="1" s="9">
+    <row r="4" ht="21.75" customHeight="1" s="10">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>21-1-00089</t>
@@ -709,7 +718,7 @@
       <c r="AI4" s="2" t="n"/>
       <c r="AJ4" s="8" t="n"/>
     </row>
-    <row r="5" ht="21.75" customHeight="1" s="9">
+    <row r="5" ht="21.75" customHeight="1" s="10">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>19-1-02014</t>
@@ -755,7 +764,7 @@
       <c r="AI5" s="2" t="n"/>
       <c r="AJ5" s="8" t="n"/>
     </row>
-    <row r="6" ht="21.75" customHeight="1" s="9">
+    <row r="6" ht="21.75" customHeight="1" s="10">
       <c r="A6" s="3" t="inlineStr">
         <is>
           <t>21-1-02414</t>
@@ -801,7 +810,7 @@
       <c r="AI6" s="2" t="n"/>
       <c r="AJ6" s="8" t="n"/>
     </row>
-    <row r="7" ht="21.75" customHeight="1" s="9">
+    <row r="7" ht="21.75" customHeight="1" s="10">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>21-1-00415</t>
@@ -847,7 +856,7 @@
       <c r="AI7" s="2" t="n"/>
       <c r="AJ7" s="8" t="n"/>
     </row>
-    <row r="8" ht="21.75" customHeight="1" s="9">
+    <row r="8" ht="21.75" customHeight="1" s="10">
       <c r="A8" s="3" t="inlineStr">
         <is>
           <t>21-1-00682</t>
@@ -893,7 +902,7 @@
       <c r="AI8" s="2" t="n"/>
       <c r="AJ8" s="8" t="n"/>
     </row>
-    <row r="9" ht="21.75" customHeight="1" s="9">
+    <row r="9" ht="21.75" customHeight="1" s="10">
       <c r="A9" s="3" t="inlineStr">
         <is>
           <t>21-1-01652</t>
@@ -939,7 +948,7 @@
       <c r="AI9" s="2" t="n"/>
       <c r="AJ9" s="8" t="n"/>
     </row>
-    <row r="10" ht="21.75" customHeight="1" s="9">
+    <row r="10" ht="21.75" customHeight="1" s="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
           <t>21-1-00161</t>
@@ -985,7 +994,7 @@
       <c r="AI10" s="2" t="n"/>
       <c r="AJ10" s="8" t="n"/>
     </row>
-    <row r="11" ht="21.75" customHeight="1" s="9">
+    <row r="11" ht="21.75" customHeight="1" s="10">
       <c r="A11" s="3" t="inlineStr">
         <is>
           <t>21-1-02462</t>
@@ -1031,7 +1040,7 @@
       <c r="AI11" s="2" t="n"/>
       <c r="AJ11" s="8" t="n"/>
     </row>
-    <row r="12" ht="21.75" customHeight="1" s="9">
+    <row r="12" ht="21.75" customHeight="1" s="10">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>21-1-01558</t>
@@ -1077,7 +1086,7 @@
       <c r="AI12" s="2" t="n"/>
       <c r="AJ12" s="8" t="n"/>
     </row>
-    <row r="13" ht="21.75" customHeight="1" s="9">
+    <row r="13" ht="21.75" customHeight="1" s="10">
       <c r="A13" s="8" t="inlineStr">
         <is>
           <t>20-1-01806</t>
@@ -1123,7 +1132,7 @@
       <c r="AI13" s="2" t="n"/>
       <c r="AJ13" s="8" t="n"/>
     </row>
-    <row r="14" ht="21.75" customHeight="1" s="9">
+    <row r="14" ht="21.75" customHeight="1" s="10">
       <c r="A14" s="8" t="inlineStr">
         <is>
           <t>21-1-00472</t>
@@ -1169,7 +1178,7 @@
       <c r="AI14" s="2" t="n"/>
       <c r="AJ14" s="8" t="n"/>
     </row>
-    <row r="15" ht="21.75" customHeight="1" s="9">
+    <row r="15" ht="21.75" customHeight="1" s="10">
       <c r="A15" s="8" t="inlineStr">
         <is>
           <t>19-1-01014</t>
@@ -1215,7 +1224,7 @@
       <c r="AI15" s="2" t="n"/>
       <c r="AJ15" s="8" t="n"/>
     </row>
-    <row r="16" ht="21.75" customHeight="1" s="9">
+    <row r="16" ht="21.75" customHeight="1" s="10">
       <c r="A16" s="8" t="inlineStr">
         <is>
           <t>21-1-02772</t>
@@ -1261,7 +1270,7 @@
       <c r="AI16" s="2" t="n"/>
       <c r="AJ16" s="8" t="n"/>
     </row>
-    <row r="17" ht="21.75" customHeight="1" s="9">
+    <row r="17" ht="21.75" customHeight="1" s="10">
       <c r="A17" s="8" t="inlineStr">
         <is>
           <t>21-1-01823</t>
@@ -1272,9 +1281,7 @@
           <t>Ramada, Avril</t>
         </is>
       </c>
-      <c r="C17" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="C17" s="8" t="n"/>
       <c r="D17" s="8" t="n"/>
       <c r="E17" s="8" t="n"/>
       <c r="F17" s="8" t="n"/>
@@ -1309,7 +1316,7 @@
       <c r="AI17" s="2" t="n"/>
       <c r="AJ17" s="8" t="n"/>
     </row>
-    <row r="18" ht="21.75" customHeight="1" s="9">
+    <row r="18" ht="21.75" customHeight="1" s="10">
       <c r="A18" s="8" t="inlineStr">
         <is>
           <t>19-1-02034</t>
@@ -1321,7 +1328,7 @@
         </is>
       </c>
       <c r="C18" s="8" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D18" s="8" t="n"/>
       <c r="E18" s="8" t="n"/>
@@ -1357,7 +1364,7 @@
       <c r="AI18" s="2" t="n"/>
       <c r="AJ18" s="8" t="n"/>
     </row>
-    <row r="19" ht="21.75" customHeight="1" s="9">
+    <row r="19" ht="21.75" customHeight="1" s="10">
       <c r="A19" s="8" t="inlineStr">
         <is>
           <t>21-1-02499</t>
@@ -1403,7 +1410,7 @@
       <c r="AI19" s="2" t="n"/>
       <c r="AJ19" s="8" t="n"/>
     </row>
-    <row r="20" ht="21.75" customHeight="1" s="9">
+    <row r="20" ht="21.75" customHeight="1" s="10">
       <c r="A20" s="8" t="inlineStr">
         <is>
           <t>21-1-00846</t>
@@ -1449,7 +1456,7 @@
       <c r="AI20" s="2" t="n"/>
       <c r="AJ20" s="8" t="n"/>
     </row>
-    <row r="21" ht="21.75" customHeight="1" s="9">
+    <row r="21" ht="21.75" customHeight="1" s="10">
       <c r="A21" s="8" t="inlineStr">
         <is>
           <t>21-1-01482</t>
@@ -1495,7 +1502,7 @@
       <c r="AI21" s="2" t="n"/>
       <c r="AJ21" s="8" t="n"/>
     </row>
-    <row r="22" ht="21.75" customHeight="1" s="9">
+    <row r="22" ht="21.75" customHeight="1" s="10">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>21-1-00870</t>
@@ -1541,7 +1548,7 @@
       <c r="AI22" s="2" t="n"/>
       <c r="AJ22" s="8" t="n"/>
     </row>
-    <row r="23" ht="21.75" customHeight="1" s="9">
+    <row r="23" ht="21.75" customHeight="1" s="10">
       <c r="A23" s="8" t="inlineStr">
         <is>
           <t>20-1-00163</t>
@@ -1587,7 +1594,7 @@
       <c r="AI23" s="2" t="n"/>
       <c r="AJ23" s="8" t="n"/>
     </row>
-    <row r="24" ht="21.75" customHeight="1" s="9">
+    <row r="24" ht="21.75" customHeight="1" s="10">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>15-1-02342</t>
@@ -1598,9 +1605,7 @@
           <t>biyatch</t>
         </is>
       </c>
-      <c r="C24" s="8" t="n">
-        <v>6</v>
-      </c>
+      <c r="C24" s="8" t="n"/>
       <c r="D24" s="8" t="n"/>
       <c r="E24" s="8" t="n"/>
       <c r="F24" s="8" t="n"/>
@@ -1635,7 +1640,7 @@
       <c r="AI24" s="2" t="n"/>
       <c r="AJ24" s="8" t="n"/>
     </row>
-    <row r="25" ht="21.75" customHeight="1" s="9">
+    <row r="25" ht="21.75" customHeight="1" s="10">
       <c r="B25" s="8" t="n"/>
       <c r="C25" s="8" t="n"/>
       <c r="D25" s="2" t="n"/>
@@ -1672,7 +1677,7 @@
       <c r="AI25" s="8" t="n"/>
       <c r="AJ25" s="8" t="n"/>
     </row>
-    <row r="26" ht="21.75" customHeight="1" s="9">
+    <row r="26" ht="21.75" customHeight="1" s="10">
       <c r="B26" s="8" t="n"/>
       <c r="C26" s="8" t="n"/>
       <c r="D26" s="2" t="n"/>
@@ -1709,7 +1714,7 @@
       <c r="AI26" s="8" t="n"/>
       <c r="AJ26" s="8" t="n"/>
     </row>
-    <row r="27" ht="21.75" customHeight="1" s="9">
+    <row r="27" ht="21.75" customHeight="1" s="10">
       <c r="B27" s="8" t="n"/>
       <c r="C27" s="8" t="n"/>
       <c r="D27" s="2" t="n"/>
@@ -1746,7 +1751,7 @@
       <c r="AI27" s="8" t="n"/>
       <c r="AJ27" s="8" t="n"/>
     </row>
-    <row r="28" ht="21.75" customHeight="1" s="9">
+    <row r="28" ht="21.75" customHeight="1" s="10">
       <c r="B28" s="8" t="n"/>
       <c r="C28" s="8" t="n"/>
       <c r="D28" s="2" t="n"/>
@@ -1783,7 +1788,7 @@
       <c r="AI28" s="8" t="n"/>
       <c r="AJ28" s="8" t="n"/>
     </row>
-    <row r="29" ht="21.75" customHeight="1" s="9">
+    <row r="29" ht="21.75" customHeight="1" s="10">
       <c r="B29" s="8" t="n"/>
       <c r="C29" s="8" t="n"/>
       <c r="D29" s="2" t="n"/>
@@ -1820,7 +1825,7 @@
       <c r="AI29" s="8" t="n"/>
       <c r="AJ29" s="8" t="n"/>
     </row>
-    <row r="30" ht="21.75" customHeight="1" s="9">
+    <row r="30" ht="21.75" customHeight="1" s="10">
       <c r="B30" s="8" t="n"/>
       <c r="C30" s="8" t="n"/>
       <c r="D30" s="2" t="n"/>
@@ -1857,7 +1862,7 @@
       <c r="AI30" s="8" t="n"/>
       <c r="AJ30" s="8" t="n"/>
     </row>
-    <row r="31" ht="21.75" customHeight="1" s="9">
+    <row r="31" ht="21.75" customHeight="1" s="10">
       <c r="B31" s="8" t="n"/>
       <c r="C31" s="8" t="n"/>
       <c r="D31" s="2" t="n"/>
@@ -1894,7 +1899,7 @@
       <c r="AI31" s="8" t="n"/>
       <c r="AJ31" s="8" t="n"/>
     </row>
-    <row r="32" ht="21.75" customHeight="1" s="9">
+    <row r="32" ht="21.75" customHeight="1" s="10">
       <c r="B32" s="8" t="n"/>
       <c r="C32" s="8" t="n"/>
       <c r="D32" s="8" t="n"/>
@@ -1931,7 +1936,7 @@
       <c r="AI32" s="8" t="n"/>
       <c r="AJ32" s="8" t="n"/>
     </row>
-    <row r="33" ht="21.75" customHeight="1" s="9">
+    <row r="33" ht="21.75" customHeight="1" s="10">
       <c r="B33" s="8" t="n"/>
       <c r="C33" s="8" t="n"/>
       <c r="D33" s="8" t="n"/>
@@ -1968,7 +1973,7 @@
       <c r="AI33" s="8" t="n"/>
       <c r="AJ33" s="8" t="n"/>
     </row>
-    <row r="34" ht="21.75" customHeight="1" s="9">
+    <row r="34" ht="21.75" customHeight="1" s="10">
       <c r="B34" s="8" t="n"/>
       <c r="C34" s="8" t="n"/>
       <c r="D34" s="8" t="n"/>
@@ -2005,7 +2010,7 @@
       <c r="AI34" s="8" t="n"/>
       <c r="AJ34" s="8" t="n"/>
     </row>
-    <row r="35" ht="21.75" customHeight="1" s="9">
+    <row r="35" ht="21.75" customHeight="1" s="10">
       <c r="B35" s="8" t="n"/>
       <c r="C35" s="8" t="n"/>
       <c r="D35" s="8" t="n"/>
@@ -2042,7 +2047,7 @@
       <c r="AI35" s="8" t="n"/>
       <c r="AJ35" s="8" t="n"/>
     </row>
-    <row r="36" ht="21.75" customHeight="1" s="9">
+    <row r="36" ht="21.75" customHeight="1" s="10">
       <c r="B36" s="8" t="n"/>
       <c r="C36" s="8" t="n"/>
       <c r="D36" s="8" t="n"/>
@@ -2079,7 +2084,7 @@
       <c r="AI36" s="8" t="n"/>
       <c r="AJ36" s="8" t="n"/>
     </row>
-    <row r="37" ht="21.75" customHeight="1" s="9">
+    <row r="37" ht="21.75" customHeight="1" s="10">
       <c r="B37" s="8" t="n"/>
       <c r="C37" s="8" t="n"/>
       <c r="D37" s="8" t="n"/>
@@ -2116,7 +2121,7 @@
       <c r="AI37" s="8" t="n"/>
       <c r="AJ37" s="8" t="n"/>
     </row>
-    <row r="38" ht="21.75" customHeight="1" s="9">
+    <row r="38" ht="21.75" customHeight="1" s="10">
       <c r="B38" s="8" t="n"/>
       <c r="C38" s="8" t="n"/>
       <c r="D38" s="8" t="n"/>
@@ -2153,7 +2158,7 @@
       <c r="AI38" s="8" t="n"/>
       <c r="AJ38" s="8" t="n"/>
     </row>
-    <row r="39" ht="21.75" customHeight="1" s="9">
+    <row r="39" ht="21.75" customHeight="1" s="10">
       <c r="B39" s="8" t="n"/>
       <c r="C39" s="8" t="n"/>
       <c r="D39" s="8" t="n"/>
@@ -2190,7 +2195,7 @@
       <c r="AI39" s="8" t="n"/>
       <c r="AJ39" s="8" t="n"/>
     </row>
-    <row r="40" ht="21.75" customHeight="1" s="9">
+    <row r="40" ht="21.75" customHeight="1" s="10">
       <c r="B40" s="8" t="n"/>
       <c r="C40" s="8" t="n"/>
       <c r="D40" s="8" t="n"/>
@@ -2227,7 +2232,7 @@
       <c r="AI40" s="8" t="n"/>
       <c r="AJ40" s="8" t="n"/>
     </row>
-    <row r="41" ht="21.75" customHeight="1" s="9">
+    <row r="41" ht="21.75" customHeight="1" s="10">
       <c r="B41" s="8" t="n"/>
       <c r="C41" s="8" t="n"/>
       <c r="D41" s="8" t="n"/>
@@ -2264,7 +2269,7 @@
       <c r="AI41" s="8" t="n"/>
       <c r="AJ41" s="8" t="n"/>
     </row>
-    <row r="42" ht="21.75" customHeight="1" s="9">
+    <row r="42" ht="21.75" customHeight="1" s="10">
       <c r="B42" s="8" t="n"/>
       <c r="C42" s="8" t="n"/>
       <c r="D42" s="8" t="n"/>
@@ -2301,7 +2306,7 @@
       <c r="AI42" s="8" t="n"/>
       <c r="AJ42" s="8" t="n"/>
     </row>
-    <row r="43" ht="21.75" customHeight="1" s="9">
+    <row r="43" ht="21.75" customHeight="1" s="10">
       <c r="B43" s="8" t="n"/>
       <c r="C43" s="8" t="n"/>
       <c r="D43" s="8" t="n"/>
@@ -2338,7 +2343,7 @@
       <c r="AI43" s="8" t="n"/>
       <c r="AJ43" s="8" t="n"/>
     </row>
-    <row r="44" ht="21.75" customHeight="1" s="9">
+    <row r="44" ht="21.75" customHeight="1" s="10">
       <c r="B44" s="8" t="n"/>
       <c r="C44" s="8" t="n"/>
       <c r="D44" s="8" t="n"/>
@@ -2375,7 +2380,7 @@
       <c r="AI44" s="8" t="n"/>
       <c r="AJ44" s="8" t="n"/>
     </row>
-    <row r="45" ht="21.75" customHeight="1" s="9">
+    <row r="45" ht="21.75" customHeight="1" s="10">
       <c r="B45" s="8" t="n"/>
       <c r="C45" s="8" t="n"/>
       <c r="D45" s="8" t="n"/>
@@ -2412,7 +2417,7 @@
       <c r="AI45" s="8" t="n"/>
       <c r="AJ45" s="8" t="n"/>
     </row>
-    <row r="46" ht="21.75" customHeight="1" s="9">
+    <row r="46" ht="21.75" customHeight="1" s="10">
       <c r="B46" s="8" t="n"/>
       <c r="C46" s="8" t="n"/>
       <c r="D46" s="8" t="n"/>
@@ -2449,7 +2454,7 @@
       <c r="AI46" s="8" t="n"/>
       <c r="AJ46" s="8" t="n"/>
     </row>
-    <row r="47" ht="21.75" customHeight="1" s="9">
+    <row r="47" ht="21.75" customHeight="1" s="10">
       <c r="B47" s="8" t="n"/>
       <c r="C47" s="8" t="n"/>
       <c r="D47" s="8" t="n"/>
@@ -2486,7 +2491,7 @@
       <c r="AI47" s="8" t="n"/>
       <c r="AJ47" s="8" t="n"/>
     </row>
-    <row r="48" ht="21.75" customHeight="1" s="9">
+    <row r="48" ht="21.75" customHeight="1" s="10">
       <c r="B48" s="8" t="n"/>
       <c r="C48" s="8" t="n"/>
       <c r="D48" s="8" t="n"/>
@@ -2535,20 +2540,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="48.7265625" customWidth="1" style="9" min="1" max="1"/>
-    <col width="14.1796875" customWidth="1" style="9" min="2" max="2"/>
-    <col width="11.26953125" customWidth="1" style="9" min="3" max="3"/>
-    <col width="11.6328125" customWidth="1" style="9" min="4" max="4"/>
-    <col width="11.453125" customWidth="1" style="9" min="5" max="5"/>
-    <col width="11.08984375" customWidth="1" style="9" min="6" max="6"/>
+    <col width="64.54296875" customWidth="1" style="10" min="1" max="1"/>
+    <col width="14.1796875" customWidth="1" style="10" min="2" max="2"/>
+    <col width="11.26953125" customWidth="1" style="10" min="3" max="3"/>
+    <col width="11.6328125" customWidth="1" style="10" min="4" max="4"/>
+    <col width="11.453125" customWidth="1" style="10" min="5" max="5"/>
+    <col width="11.08984375" customWidth="1" style="10" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2562,274 +2567,205 @@
           <t>CHOICE A</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>CHOICE B</t>
-        </is>
-      </c>
-      <c r="D1" s="5" t="inlineStr">
-        <is>
-          <t>CHOICE C</t>
-        </is>
-      </c>
-      <c r="E1" s="5" t="inlineStr">
-        <is>
-          <t>CHOICE D</t>
-        </is>
-      </c>
-      <c r="F1" s="5" t="inlineStr">
-        <is>
-          <t>CHOICE E</t>
-        </is>
-      </c>
+      <c r="C1" s="5" t="n"/>
+      <c r="D1" s="5" t="n"/>
+      <c r="E1" s="5" t="n"/>
+      <c r="F1" s="5" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>What is 1 + 1</t>
-        </is>
-      </c>
-      <c r="B2" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5</v>
+          <t>What is the Earth's primary source of energy?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Wind</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>Solar Radiation</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Fossil fuels</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Geothermal</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>All of the Above</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>What is 2 + 2</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>69</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" t="n">
-        <v>8</v>
-      </c>
-      <c r="F3" t="n">
-        <v>10</v>
+          <t>Which planet is known as the "Red Planet"?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Venus</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>Mars</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Jupiter</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Saturn</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>All of the Above</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>What is 12 + 12</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>23</v>
-      </c>
-      <c r="C4" t="n">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="E4" t="n">
-        <v>98</v>
-      </c>
-      <c r="F4" t="n">
-        <v>28</v>
+          <t>What is the process by which plants make their own food using sunlight?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Respiration</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>Photosynthesis</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Transpiration</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Digestion</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>All of the Above</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>What is 24 + 23</t>
-        </is>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>47</v>
-      </c>
-      <c r="C5" t="n">
-        <v>45</v>
-      </c>
-      <c r="D5" t="n">
-        <v>24</v>
-      </c>
-      <c r="E5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F5" t="n">
-        <v>29</v>
+          <t>What is the smallest unit of matter?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Atom</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Molecule</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Cell</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>Electron</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>All of the Above</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>It is called the river of life</t>
+          <t>Which organ is responsible for pumping blood throughout the body?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nile River</t>
-        </is>
-      </c>
-      <c r="C6" s="6" t="inlineStr">
-        <is>
-          <t>Blood</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Pasig River</t>
+          <t>Lungs</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Liver</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>Heart</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Rivermaya</t>
+          <t>Kidneys</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Egyptian River</t>
+          <t>All of the Above</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>When is the World War I</t>
+          <t>What is the process by which water changes from a liquid to a gas?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jan. 11, 2023</t>
-        </is>
-      </c>
-      <c r="C7" s="11" t="inlineStr">
-        <is>
-          <t>Jul. 28, 1914</t>
-        </is>
-      </c>
-      <c r="D7" s="10" t="inlineStr">
-        <is>
-          <t>Dec. 11, 1998</t>
-        </is>
-      </c>
-      <c r="E7" s="10" t="n">
-        <v>38785</v>
+          <t>Freezin</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
+        <is>
+          <t>Condensation</t>
+        </is>
+      </c>
+      <c r="D7" s="12" t="inlineStr">
+        <is>
+          <t>Evaporation</t>
+        </is>
+      </c>
+      <c r="E7" s="11" t="inlineStr">
+        <is>
+          <t>Melting</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sep. 06, 1921</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>What is the chemical symbol for element Gold?</t>
-        </is>
-      </c>
-      <c r="B8" s="6" t="inlineStr">
-        <is>
-          <t>Au</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Ag</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Fe</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Hg</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>What is the capital of France?</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Madrid</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Berlin</t>
-        </is>
-      </c>
-      <c r="D9" s="6" t="inlineStr">
-        <is>
-          <t>Paris</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Rome</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Manila</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>What is the powerhouse of the cell?</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Nucleus</t>
-        </is>
-      </c>
-      <c r="C10" s="6" t="inlineStr">
-        <is>
-          <t>Mitochondria</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Endoplasmic Reticulum</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Golgi Apparatus</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>None of the Above</t>
+          <t>All of the Above</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>